<commit_message>
Edit and delete share skill added
</commit_message>
<xml_diff>
--- a/Competition/Competition/ExcelData/TestData.xlsx
+++ b/Competition/Competition/ExcelData/TestData.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Competition\Competition\Competition\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BF73D7-DEFC-434A-87E0-9B96FC924A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1A1574-87D0-4155-ADDC-CB18FB854343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
-    <sheet name="ShareSkill" sheetId="4" r:id="rId3"/>
-    <sheet name="Profile" sheetId="2" r:id="rId4"/>
+    <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="ShareSkill" sheetId="4" r:id="rId4"/>
     <sheet name="ManageListings" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
   <si>
     <t>Url</t>
   </si>
@@ -182,9 +183,6 @@
     <t>ActiveOption</t>
   </si>
   <si>
-    <t>Sql</t>
-  </si>
-  <si>
     <t>StartTime</t>
   </si>
   <si>
@@ -206,19 +204,164 @@
     <t>Online</t>
   </si>
   <si>
-    <t>Deleteaction</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Telugu Language</t>
+  </si>
+  <si>
+    <t>I would like to share Telugu Language skills.</t>
+  </si>
+  <si>
+    <t>Writing &amp; Translation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Writing, Reading,Speaking</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>08:00AM</t>
+  </si>
+  <si>
+    <t>06:00PM</t>
+  </si>
+  <si>
+    <t>TC ID</t>
+  </si>
+  <si>
+    <t>DeleteAction</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Presentations</t>
+  </si>
+  <si>
+    <t>Spring Planning, Sprint Review</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>07:00AM</t>
+  </si>
+  <si>
+    <t>05:00PM</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>SpecFlow</t>
+  </si>
+  <si>
+    <t>Video Marketing</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>I would like to share about spec flow BDD.</t>
+  </si>
+  <si>
+    <t>I would like to share about agile scrum ceremonies.</t>
+  </si>
+  <si>
+    <t>Feature file, StepDefinitions</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>9:00AM</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Beauty Services</t>
+  </si>
+  <si>
+    <t>Healthy Habits</t>
+  </si>
+  <si>
+    <t>I want to share eating haelthy food and doing exercise.</t>
+  </si>
+  <si>
+    <t>I want share about mackup tips and nail art.</t>
+  </si>
+  <si>
+    <t>Fun &amp; Lifestyle</t>
+  </si>
+  <si>
+    <t>Health, Nutrition &amp; Fitness</t>
+  </si>
+  <si>
+    <t>Online Lessons</t>
+  </si>
+  <si>
+    <t>Mackup, Nailart</t>
+  </si>
+  <si>
+    <t>Healthy Diet, Exercise</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>09:00AM</t>
+  </si>
+  <si>
+    <t>08:00PM</t>
+  </si>
+  <si>
+    <t>Fun</t>
+  </si>
+  <si>
+    <t>Lifestyle</t>
+  </si>
+  <si>
+    <t>MEETINGS AND CEREMONIES</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Operators</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -236,7 +379,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +389,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,13 +415,25 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -615,7 +776,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,139 +881,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DFDA03-AA45-4BE3-9A3F-FBBD946DFB85}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="3">
-        <v>44788</v>
-      </c>
-      <c r="I2" s="4">
-        <v>44804</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="M2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -941,38 +969,654 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14355D16-8D87-4C9D-B05A-D8A1B31AF3AB}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DFDA03-AA45-4BE3-9A3F-FBBD946DFB85}">
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="11">
+        <v>44832</v>
+      </c>
+      <c r="I2" s="11">
+        <v>44863</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="11">
+        <v>44829</v>
+      </c>
+      <c r="I3" s="11">
+        <v>44852</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="11">
+        <v>44826</v>
+      </c>
+      <c r="I4" s="11">
+        <v>44856</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="11">
+        <v>44815</v>
+      </c>
+      <c r="I5" s="11">
+        <v>44852</v>
+      </c>
+      <c r="J5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5">
+        <v>7</v>
+      </c>
+      <c r="P5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I11" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14355D16-8D87-4C9D-B05A-D8A1B31AF3AB}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="11">
+        <v>44829</v>
+      </c>
+      <c r="J5" s="11">
+        <v>44862</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="11">
+        <v>44828</v>
+      </c>
+      <c r="J6" s="11">
+        <v>44853</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="11">
+        <v>44828</v>
+      </c>
+      <c r="J7" s="11">
+        <v>44854</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" t="s">
+        <v>102</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD01B95F-97B9-4344-B08D-E54AAC879DDA}">
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add, Edit, Delete, and Invalid TCs added
</commit_message>
<xml_diff>
--- a/Competition/Competition/ExcelData/TestData.xlsx
+++ b/Competition/Competition/ExcelData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Competition\Competition\Competition\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1A1574-87D0-4155-ADDC-CB18FB854343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AF0BDA-C1E5-4CFD-BA91-6C9729F8AE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Profile" sheetId="2" r:id="rId3"/>
     <sheet name="ShareSkill" sheetId="4" r:id="rId4"/>
     <sheet name="ManageListings" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="InvalidTest" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="121">
   <si>
     <t>Url</t>
   </si>
@@ -147,12 +147,6 @@
     <t>LocationType</t>
   </si>
   <si>
-    <t>Startdate</t>
-  </si>
-  <si>
-    <t>Enddate</t>
-  </si>
-  <si>
     <t>SkillTrade</t>
   </si>
   <si>
@@ -246,12 +240,6 @@
     <t>Spring Planning, Sprint Review</t>
   </si>
   <si>
-    <t>Hourly basis service</t>
-  </si>
-  <si>
-    <t>On-site</t>
-  </si>
-  <si>
     <t>Mon</t>
   </si>
   <si>
@@ -264,36 +252,9 @@
     <t>Hidden</t>
   </si>
   <si>
-    <t>SpecFlow</t>
-  </si>
-  <si>
-    <t>Video Marketing</t>
-  </si>
-  <si>
-    <t>Digital Marketing</t>
-  </si>
-  <si>
-    <t>I would like to share about spec flow BDD.</t>
-  </si>
-  <si>
     <t>I would like to share about agile scrum ceremonies.</t>
   </si>
   <si>
-    <t>Feature file, StepDefinitions</t>
-  </si>
-  <si>
-    <t>Thu</t>
-  </si>
-  <si>
-    <t>9:00AM</t>
-  </si>
-  <si>
-    <t>6:00PM</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Beauty Services</t>
   </si>
   <si>
@@ -315,9 +276,6 @@
     <t>Online Lessons</t>
   </si>
   <si>
-    <t>Mackup, Nailart</t>
-  </si>
-  <si>
     <t>Healthy Diet, Exercise</t>
   </si>
   <si>
@@ -342,9 +300,6 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -352,6 +307,94 @@
   </si>
   <si>
     <t>Operators</t>
+  </si>
+  <si>
+    <t>TC-1</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Agile Methodology &amp; SQL queries</t>
+  </si>
+  <si>
+    <t>ErrorMessages</t>
+  </si>
+  <si>
+    <t>Special characters are not allowed.</t>
+  </si>
+  <si>
+    <t>I would like to share about @agile scrum
+ topics &amp; basic @ SQL queries.</t>
+  </si>
+  <si>
+    <t>Subcategory is required</t>
+  </si>
+  <si>
+    <t>ClickSave</t>
+  </si>
+  <si>
+    <t>Tag is required</t>
+  </si>
+  <si>
+    <t>Please complete 
+the form correctly.</t>
+  </si>
+  <si>
+    <t>Tags are required</t>
+  </si>
+  <si>
+    <t>Start Date cannot
+ be set to a day in the past</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Start Date cannot 
+be set to a day in
+ the past</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>TC-2</t>
+  </si>
+  <si>
+    <t>&gt;Agile Methodology and &gt;SQL queries</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>First character must be an
+ alphabet character or a number.</t>
+  </si>
+  <si>
+    <t>I would like to share about 
+Agile Methodology &amp; SQL Queries.</t>
+  </si>
+  <si>
+    <t>Category is required</t>
+  </si>
+  <si>
+    <t>Telugu Writing and Translation</t>
+  </si>
+  <si>
+    <t>Creative Writing</t>
+  </si>
+  <si>
+    <t>Join Operator</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>Mackup</t>
   </si>
 </sst>
 </file>
@@ -363,7 +406,7 @@
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,8 +421,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFDB2828"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,13 +448,40 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -415,7 +492,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -434,6 +511,37 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -971,15 +1079,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DFDA03-AA45-4BE3-9A3F-FBBD946DFB85}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="2" max="2" width="60.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
@@ -1007,7 +1115,7 @@
         <v>36</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>37</v>
@@ -1019,22 +1127,22 @@
         <v>39</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="L1" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>33</v>
@@ -1043,31 +1151,31 @@
         <v>34</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="11">
         <v>44832</v>
@@ -1076,48 +1184,48 @@
         <v>44863</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
         <v>55</v>
       </c>
-      <c r="M2" t="s">
-        <v>57</v>
-      </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="O2">
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="11">
         <v>44829</v>
@@ -1126,16 +1234,16 @@
         <v>44852</v>
       </c>
       <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" t="s">
         <v>65</v>
       </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
         <v>3</v>
@@ -1144,135 +1252,35 @@
         <v>5</v>
       </c>
       <c r="P3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="11">
-        <v>44826</v>
-      </c>
-      <c r="I4" s="11">
-        <v>44856</v>
-      </c>
-      <c r="J4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" t="s">
-        <v>104</v>
-      </c>
-      <c r="O4">
-        <v>5</v>
-      </c>
-      <c r="P4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="11">
-        <v>44815</v>
-      </c>
-      <c r="I5" s="11">
-        <v>44852</v>
-      </c>
-      <c r="J5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" t="s">
-        <v>86</v>
-      </c>
-      <c r="L5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5">
-        <v>7</v>
-      </c>
-      <c r="P5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I9" s="7"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="8"/>
-      <c r="F13" s="3"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1282,20 +1290,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14355D16-8D87-4C9D-B05A-D8A1B31AF3AB}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="4" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
@@ -1307,7 +1314,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>35</v>
@@ -1319,7 +1326,7 @@
         <v>36</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>37</v>
@@ -1331,22 +1338,22 @@
         <v>39</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="M1" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>33</v>
@@ -1355,58 +1362,193 @@
         <v>34</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="11">
+        <v>44832</v>
+      </c>
+      <c r="J2" s="11">
+        <v>44863</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s">
-        <v>62</v>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="11">
+        <v>44829</v>
+      </c>
+      <c r="J3" s="11">
+        <v>44852</v>
+      </c>
+      <c r="K3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="11">
+        <v>44828</v>
+      </c>
+      <c r="J4" s="11">
+        <v>44853</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
         <v>70</v>
       </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="I5" s="11">
         <v>44829</v>
@@ -1415,136 +1557,79 @@
         <v>44862</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="M5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N5" t="s">
         <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="P5">
         <v>5</v>
       </c>
       <c r="Q5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I6" s="11">
         <v>44828</v>
       </c>
       <c r="J6" s="11">
-        <v>44853</v>
+        <v>44854</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O6" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="P6">
         <v>5</v>
       </c>
       <c r="Q6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="11">
-        <v>44828</v>
-      </c>
-      <c r="J7" s="11">
-        <v>44854</v>
-      </c>
-      <c r="K7" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" t="s">
-        <v>99</v>
-      </c>
-      <c r="M7" t="s">
-        <v>100</v>
-      </c>
-      <c r="N7" t="s">
-        <v>57</v>
-      </c>
-      <c r="O7" t="s">
-        <v>102</v>
-      </c>
-      <c r="P7">
-        <v>5</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1554,69 +1639,274 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD01B95F-97B9-4344-B08D-E54AAC879DDA}">
-  <dimension ref="A1:R1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="15">
+        <v>44791</v>
+      </c>
+      <c r="I2" s="15">
+        <v>44790</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="24">
+        <v>44788</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="23">
+        <v>15</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="21" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>